<commit_message>
add component indicators and list user, add assesor
</commit_message>
<xml_diff>
--- a/formatExcel/Assoc_Indicator.xlsx
+++ b/formatExcel/Assoc_Indicator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilson/PhpstormProjects/plannerapp/formatExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F6FA1E-8AE1-1347-B91E-3E0F4D21B97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DACF88D-5E2D-6543-BDEC-3984B9FDF7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{D6733E99-025E-414C-AF63-B97D3ACFA750}"/>
+    <workbookView xWindow="6520" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{D6733E99-025E-414C-AF63-B97D3ACFA750}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,7 +461,7 @@
         <v>2024</v>
       </c>
       <c r="B2">
-        <v>146</v>
+        <v>849</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -475,5 +475,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>